<commit_message>
Se sustrajo todo el contenido relacionado con RootNode. Se agregaron cambios a blogs Meshtastic, así como la creación de nuevos.
</commit_message>
<xml_diff>
--- a/blog/datos.xlsx
+++ b/blog/datos.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="Batería" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Costos" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Cronología" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -145,6 +146,7 @@
     <author>tc={09D56106-0768-0620-F096-C8788256A593}</author>
     <author>tc={CF5B2ACF-561A-1DE4-B3F1-814FFF68FBC8}</author>
     <author>tc={58F1B934-F0EC-B8A6-F92F-6925362D7875}</author>
+    <author>tc={323C15CB-F46B-052A-11E0-662EF2810C65}</author>
   </authors>
   <commentList>
     <comment ref="D3" authorId="0" xr:uid="{09D56106-0768-0620-F096-C8788256A593}">
@@ -210,12 +212,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="A9" authorId="3" xr:uid="{323C15CB-F46B-052A-11E0-662EF2810C65}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>pablovo-t470s:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Compra conjunta al M6
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Mediciones</t>
   </si>
@@ -359,6 +382,180 @@
   </si>
   <si>
     <t xml:space="preserve">ThinkNode M6</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N° de compra</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Suceso</t>
+  </si>
+  <si>
+    <t>Elecrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 3M1 y 2M6 desde la página oficial de Elecrow. Se estima que llegue entre el 11/12/25 y el 16/12/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reintegro de 37 U$D por cambio de courier (FedEx a HK-DHL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despachó el paquete. Envío via HK-DHL y se estima que llegue entre 14/01/26 y el 17/01/26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingreso a aduana + Pago de impuestos ($126.890,40)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paquete recibido.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 3M1 desde la página oficial de Elecrow. Se estima que llegue entre el 15/12/25 y el 19/12/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despachó el paquete. Envío via HK-DHL y se estima que llegue entre 14/12/25 y el 17/12/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingreso a aduana + Pago de impuestos ($44.915,97).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intento fallido de entrega, se deberá retirar en sucursal (Ayacucho 53 - Cba.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compra de 3 M5 Pro. Se estima que llegue entre el 13/01/26 y el 16/01/26. Envío vía DHL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Despacho del paquete. Envío vía DHL. Se estima que llegue el 31/01/26</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ingreso a aduana + Pago de impuestos ($71.142,17)</t>
+  </si>
+  <si>
+    <t>Heltec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 2 pack (1 amarillo y 1 gris) MeshPocket Qi2 (6u.) desde la página oficial de Heltec. Se estima que llegue entre 11/12/25 y el 16/12/25.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra cancelada desde Heltec, sin motivos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reintegro por la cancelación de nuestra compra. Desición unilateral de la empresa Heltec.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 2 pack (1 amarillo y 1 gris) de 3 MeshPocket Qi2 (6u.) desde la página oficial de Heltec. Sin fecha estimada de entrega.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra cancelada desde Elecrow, por altos cargos de envío.</t>
+  </si>
+  <si>
+    <t>LilyGo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 3 T-Deck. </t>
+  </si>
+  <si>
+    <t>Meshnology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 1 pack N37 (2u.) por Amazon. Se estima que llegue el 23/12/25.  Se pagaron impuestos, cargos por importación e IVA total incluido. Vía Amazon priority shipping. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedido cancelado porque no pudo completar el pago. No habrá reintegro, porque no se debitó el monto de la compra.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 2 pack N37 (4u.) por Amazon. Se estima que llegue el 30/12/25. Se pagaron impuestos, cargos por importación e IVA total incluido, sin embargo no se pagó envío. Vía Amazon standar shipping.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paquete recibido. No se notificó cuándo entro al país, tampoco se pagaron impuestos posteriormente ya que los pagamos al momento de efectuar la compra en Amazon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 1 pack N37 (2u.), color rosa, por Amazon. Sin fecha estimada de llegada, vía Amazon global estandar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra cancelada. Dada la baja calidad del producto, se decidió dar de baja la compra. No hubo reintegro por la cancelación de la compra debido a que no se debitó el monto de la misma.</t>
+  </si>
+  <si>
+    <t>RAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 3 WisMesh Tag desde AliExpress. Se estima que llegue el 26/12/25.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despacho del paquete. Envío vía DHL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingreso a aduana + Pago de impuestos ($47.394,49).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paquete recibido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 3 WisMesh Tag desde RAK. Sin estimación de fecha de entrega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despacho del paquete. Envío vía DHL y se estima que llegue el 19/12/25.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingreso a aduana + Pago de impuestos ($216.634,30).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paquete retirado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solicitud de reintegro por cobro erróneo de impuestos aduaneros por parte de DHL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reintegro por cobro erróneo de impuestos aduaneros por parte de DHL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seed Studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 2 P1 a través de la página oficial de Seedstudio. Se estima que llegue entre 14/12/25 y el 18/12/25.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despacho del paquete. Envío vía FedEx.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrega de paquete + pago de impuestos ($141.428,97)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 3 Wio Tracker L1 Pro. Se estima que llegue entre 09/01/26 y el 14/01/26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despacho del paquete.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingreso a Aduana + Pago de impuestos ($81.688,40)</t>
+  </si>
+  <si>
+    <t>Spec5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra de 1 Voyager. Se estima que llegue el 22/12/25 a los depósitos de AeroBox en EEUU.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despacho del paquete. Envío vía USPS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arribo del paquete a los depósitos de Aerobox en Miami.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solicitud de envío del paquete desde Miami a Argentina.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despacho del paquete hacia Argentina. Se estima que llegue el 02/01/26.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arribo del paquete a Argentina.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pago a Aerobox ($137.659,50) + Envío vía Andreani.</t>
   </si>
 </sst>
 </file>
@@ -403,7 +600,7 @@
       <name val="Hack Nerd Font"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,8 +658,14 @@
         <bgColor theme="1" tint="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="2"/>
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="23">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -539,12 +742,197 @@
       </bottom>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right style="mediumDashDotDot">
+        <color theme="1"/>
+      </right>
+      <top style="mediumDashDotDot">
+        <color theme="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right style="mediumDashDotDot">
+        <color theme="1"/>
+      </right>
+      <top style="mediumDashDotDot">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right style="none"/>
+      <top style="mediumDashDotDot">
+        <color theme="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="mediumDashDotDot">
+        <color theme="1"/>
+      </right>
+      <top style="mediumDashDotDot">
+        <color theme="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right style="mediumDashDotDot">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="mediumDashDotDot">
+        <color theme="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="mediumDashDotDot">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="mediumDashDotDot">
+        <color theme="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="mediumDashDotDot">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="mediumDashDotDot">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right style="mediumDashDotDot">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="mediumDashDotDot">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="mediumDashDotDot">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="mediumDashDotDot">
+        <color theme="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right style="mediumDashDotDot">
+        <color theme="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="mediumDashDotDot">
+        <color theme="1"/>
+      </left>
+      <right style="mediumDashDotDot">
+        <color theme="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="mediumDashDotDot">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="mediumDashDotDot">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="67">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -628,6 +1016,120 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="9" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="9" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="11" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="13" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="17" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="11" borderId="13" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="11" borderId="13" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="11" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="19" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="11" borderId="22" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="20" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="21" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -647,7 +1149,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="pablovo-t470s" id="{222A78D6-13A6-8005-59C6-45A852B9E067}" userId="pablovo-t470s" providerId="Teamlab"/>
+  <person displayName="pablovo-t470s" id="{308D8EBE-8AFA-4748-D239-3C68FDEA8D60}" userId="pablovo-t470s" providerId="Teamlab"/>
 </personList>
 </file>
 
@@ -1095,26 +1597,26 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B11" dT="2026-01-14T15:51:35.02Z" personId="{222A78D6-13A6-8005-59C6-45A852B9E067}" id="{144BCBE1-AA2B-AF66-A192-8C39C2B2E6A9}" done="0">
+  <threadedComment ref="B11" dT="2026-01-14T15:51:35.02Z" personId="{308D8EBE-8AFA-4748-D239-3C68FDEA8D60}" id="{144BCBE1-AA2B-AF66-A192-8C39C2B2E6A9}" done="0">
     <text xml:space="preserve">GPS: OFF
 Bluetooth: OFF
 </text>
   </threadedComment>
-  <threadedComment ref="B12" dT="2026-01-14T15:50:58.48Z" personId="{222A78D6-13A6-8005-59C6-45A852B9E067}" id="{F01FD7B1-2F45-0B14-9972-A7554400386F}" done="0">
+  <threadedComment ref="B12" dT="2026-01-14T15:50:58.48Z" personId="{308D8EBE-8AFA-4748-D239-3C68FDEA8D60}" id="{F01FD7B1-2F45-0B14-9972-A7554400386F}" done="0">
     <text xml:space="preserve">GPS: ON
 Bluetooth: ON
 </text>
   </threadedComment>
-  <threadedComment ref="G6" dT="2026-01-14T13:54:57.22Z" personId="{222A78D6-13A6-8005-59C6-45A852B9E067}" id="{354F0676-B10D-1EF9-4F8D-5B58331E28DF}" done="0">
+  <threadedComment ref="G6" dT="2026-01-14T13:54:57.22Z" personId="{308D8EBE-8AFA-4748-D239-3C68FDEA8D60}" id="{354F0676-B10D-1EF9-4F8D-5B58331E28DF}" done="0">
     <text xml:space="preserve">Esto no es exacto, ya que fue a la hora que se vió apagado, por lo que puede que esta duración haya sido menor aún.
 </text>
   </threadedComment>
-  <threadedComment ref="B9" dT="2026-01-14T15:50:09.58Z" personId="{222A78D6-13A6-8005-59C6-45A852B9E067}" id="{5BC188A9-7734-CDFA-5E5C-04AFEC523C79}" done="0">
+  <threadedComment ref="B9" dT="2026-01-14T15:50:09.58Z" personId="{308D8EBE-8AFA-4748-D239-3C68FDEA8D60}" id="{5BC188A9-7734-CDFA-5E5C-04AFEC523C79}" done="0">
     <text xml:space="preserve">GPS: ON
 Bluetooth: OFF
 </text>
   </threadedComment>
-  <threadedComment ref="B10" dT="2026-01-14T15:52:10.75Z" personId="{222A78D6-13A6-8005-59C6-45A852B9E067}" id="{2DC46168-A174-B54A-40D6-0F62CD9062BE}" done="0">
+  <threadedComment ref="B10" dT="2026-01-14T15:52:10.75Z" personId="{308D8EBE-8AFA-4748-D239-3C68FDEA8D60}" id="{2DC46168-A174-B54A-40D6-0F62CD9062BE}" done="0">
     <text xml:space="preserve">GPS: OFF
 Bluetooth: ON
 </text>
@@ -1124,16 +1626,20 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D3" dT="2026-01-16T15:32:19.54Z" personId="{222A78D6-13A6-8005-59C6-45A852B9E067}" id="{09D56106-0768-0620-F096-C8788256A593}" done="0">
+  <threadedComment ref="D3" dT="2026-01-16T15:32:19.54Z" personId="{308D8EBE-8AFA-4748-D239-3C68FDEA8D60}" id="{09D56106-0768-0620-F096-C8788256A593}" done="0">
     <text xml:space="preserve">Sujeto a cambios. Investigación DHL
 </text>
   </threadedComment>
-  <threadedComment ref="E3" dT="2026-01-16T15:32:36.28Z" personId="{222A78D6-13A6-8005-59C6-45A852B9E067}" id="{CF5B2ACF-561A-1DE4-B3F1-814FFF68FBC8}" done="0">
+  <threadedComment ref="E3" dT="2026-01-16T15:32:36.28Z" personId="{308D8EBE-8AFA-4748-D239-3C68FDEA8D60}" id="{CF5B2ACF-561A-1DE4-B3F1-814FFF68FBC8}" done="0">
     <text xml:space="preserve">Sujeto a cambios. Investigación DHL
 </text>
   </threadedComment>
-  <threadedComment ref="G8" dT="2026-01-16T15:27:40.20Z" personId="{222A78D6-13A6-8005-59C6-45A852B9E067}" id="{58F1B934-F0EC-B8A6-F92F-6925362D7875}" done="0">
+  <threadedComment ref="G8" dT="2026-01-16T15:27:40.20Z" personId="{308D8EBE-8AFA-4748-D239-3C68FDEA8D60}" id="{58F1B934-F0EC-B8A6-F92F-6925362D7875}" done="0">
     <text xml:space="preserve">Cambio de Courier Fedex ==&gt; HK DHL
+</text>
+  </threadedComment>
+  <threadedComment ref="A9" dT="2026-01-22T16:54:51.76Z" personId="{308D8EBE-8AFA-4748-D239-3C68FDEA8D60}" id="{323C15CB-F46B-052A-11E0-662EF2810C65}" done="0">
+    <text xml:space="preserve">Compra conjunta al M6
 </text>
   </threadedComment>
 </ThreadedComments>
@@ -1492,13 +1998,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00A70053-0004-4A5D-861C-0084005D00B1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D90054-0099-4578-82F5-002100740002}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$I$4:$I$10</xm:f>
           </x14:formula1>
           <xm:sqref>A1:A3 A101:A1048576 A2:A3 A1:G1 A1:G1</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006D006F-00B6-4955-9C49-0093007E005C}" type="list" allowBlank="0" errorStyle="stop" imeMode="noControl" operator="between" promptTitle="" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008300D6-0007-4FE0-A026-0015006D0049}" type="list" allowBlank="0" errorStyle="stop" imeMode="noControl" operator="between" promptTitle="" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$I$4:$I$10</xm:f>
           </x14:formula1>
@@ -1513,7 +2019,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1597,25 +2103,25 @@
         <v>0</v>
       </c>
       <c r="H2" s="18">
-        <f>B2+C2+E2-F2-G2</f>
+        <f t="shared" ref="H2:H9" si="1">B2+C2+E2-F2-G2</f>
         <v>224.57135548172755</v>
       </c>
       <c r="I2" s="19">
         <v>3</v>
       </c>
       <c r="J2" s="20">
-        <f>H2/I2</f>
+        <f t="shared" ref="J2:J9" si="2">H2/I2</f>
         <v>74.857118493909184</v>
       </c>
       <c r="K2" s="21">
         <v>39</v>
       </c>
       <c r="L2" s="22">
-        <f>K2-J2</f>
+        <f t="shared" ref="L2:L9" si="3">K2-J2</f>
         <v>-35.857118493909184</v>
       </c>
       <c r="M2" s="23">
-        <f>J2*100/K2</f>
+        <f>(J2*100)/K2</f>
         <v>191.941329471562</v>
       </c>
     </row>
@@ -1643,25 +2149,25 @@
         <v>0</v>
       </c>
       <c r="H3" s="18">
-        <f>B3+C3+E3-F3-G3</f>
+        <f t="shared" si="1"/>
         <v>310.97305647840528</v>
       </c>
       <c r="I3" s="19">
         <v>3</v>
       </c>
       <c r="J3" s="20">
-        <f>H3/I3</f>
+        <f t="shared" si="2"/>
         <v>103.65768549280176</v>
       </c>
       <c r="K3" s="21">
         <v>39</v>
       </c>
       <c r="L3" s="22">
-        <f>K3-J3</f>
+        <f t="shared" si="3"/>
         <v>-64.657685492801761</v>
       </c>
       <c r="M3" s="23">
-        <f>J3*100/K3</f>
+        <f t="shared" ref="M3:M9" si="4">J3*100/K3</f>
         <v>265.78893716103016</v>
       </c>
     </row>
@@ -1689,25 +2195,25 @@
         <v>0</v>
       </c>
       <c r="H4" s="18">
-        <f>B4+C4+E4-F4-G4</f>
+        <f t="shared" si="1"/>
         <v>200.01144186046511</v>
       </c>
       <c r="I4" s="19">
         <v>4</v>
       </c>
       <c r="J4" s="20">
-        <f>H4/I4</f>
+        <f t="shared" si="2"/>
         <v>50.002860465116278</v>
       </c>
       <c r="K4" s="21">
         <v>49.990000000000002</v>
       </c>
       <c r="L4" s="22">
-        <f>K4-J4</f>
+        <f t="shared" si="3"/>
         <v>-0.012860465116276032</v>
       </c>
       <c r="M4" s="23">
-        <f>J4*100/K4</f>
+        <f t="shared" si="4"/>
         <v>100.02572607544765</v>
       </c>
     </row>
@@ -1735,25 +2241,25 @@
         <v>0</v>
       </c>
       <c r="H5" s="18">
-        <f>B5+C5+E5-F5-G5</f>
+        <f t="shared" si="1"/>
         <v>351.26273754152828</v>
       </c>
       <c r="I5" s="19">
         <v>2</v>
       </c>
       <c r="J5" s="20">
-        <f>H5/I5</f>
+        <f t="shared" si="2"/>
         <v>175.63136877076414</v>
       </c>
       <c r="K5" s="21">
         <v>69.900000000000006</v>
       </c>
       <c r="L5" s="22">
-        <f>K5-J5</f>
+        <f t="shared" si="3"/>
         <v>-105.73136877076413</v>
       </c>
       <c r="M5" s="23">
-        <f>J5*100/K5</f>
+        <f t="shared" si="4"/>
         <v>251.26089952899014</v>
       </c>
     </row>
@@ -1781,25 +2287,25 @@
         <v>0</v>
       </c>
       <c r="H6" s="18">
-        <f>B6+C6+E6-F6-G6</f>
+        <f t="shared" si="1"/>
         <v>231.54800664451827</v>
       </c>
       <c r="I6" s="19">
         <v>3</v>
       </c>
       <c r="J6" s="20">
-        <f>H6/I6</f>
+        <f t="shared" si="2"/>
         <v>77.182668881506089</v>
       </c>
       <c r="K6" s="21">
         <v>42.899999999999999</v>
       </c>
       <c r="L6" s="22">
-        <f>K6-J6</f>
+        <f t="shared" si="3"/>
         <v>-34.28266888150609</v>
       </c>
       <c r="M6" s="23">
-        <f>J6*100/K6</f>
+        <f t="shared" si="4"/>
         <v>179.91298107577177</v>
       </c>
     </row>
@@ -1827,25 +2333,25 @@
         <v>0</v>
       </c>
       <c r="H7" s="18">
-        <f>B7+C7+E7-F7-G7</f>
+        <f t="shared" si="1"/>
         <v>320.88933554817277</v>
       </c>
       <c r="I7" s="19">
         <v>1</v>
       </c>
       <c r="J7" s="20">
-        <f>H7/I7</f>
+        <f t="shared" si="2"/>
         <v>320.88933554817277</v>
       </c>
       <c r="K7" s="21">
         <v>219.99000000000001</v>
       </c>
       <c r="L7" s="22">
-        <f>K7-J7</f>
+        <f t="shared" si="3"/>
         <v>-100.89933554817276</v>
       </c>
       <c r="M7" s="23">
-        <f>J7*100/K7</f>
+        <f t="shared" si="4"/>
         <v>145.86541913185724</v>
       </c>
     </row>
@@ -1873,25 +2379,25 @@
         <v>37</v>
       </c>
       <c r="H8" s="18">
-        <f>B8+C8+E8-F8-G8</f>
+        <f t="shared" si="1"/>
         <v>207.66449833887043</v>
       </c>
       <c r="I8" s="19">
         <v>3</v>
       </c>
       <c r="J8" s="20">
-        <f>H8/I8</f>
+        <f t="shared" si="2"/>
         <v>69.221499446290139</v>
       </c>
       <c r="K8" s="21">
         <v>53.899999999999999</v>
       </c>
       <c r="L8" s="22">
-        <f>K8-J8</f>
+        <f t="shared" si="3"/>
         <v>-15.32149944629014</v>
       </c>
       <c r="M8" s="23">
-        <f>J8*100/K8</f>
+        <f t="shared" si="4"/>
         <v>128.42578746992604</v>
       </c>
     </row>
@@ -1919,25 +2425,25 @@
         <v>0</v>
       </c>
       <c r="H9" s="18">
-        <f>B9+C9+E9-F9-G9</f>
+        <f t="shared" si="1"/>
         <v>268.89255813953486</v>
       </c>
       <c r="I9" s="19">
         <v>3</v>
       </c>
       <c r="J9" s="20">
-        <f>H9/I9</f>
+        <f t="shared" si="2"/>
         <v>89.630852713178285</v>
       </c>
       <c r="K9" s="21">
         <v>53.899999999999999</v>
       </c>
       <c r="L9" s="22">
-        <f>K9-J9</f>
+        <f t="shared" si="3"/>
         <v>-35.730852713178287</v>
       </c>
       <c r="M9" s="23">
-        <f>J9*100/K9</f>
+        <f t="shared" si="4"/>
         <v>166.29100688901352</v>
       </c>
     </row>
@@ -1955,7 +2461,7 @@
         <v>71142.169999999998</v>
       </c>
       <c r="E10" s="17">
-        <f t="shared" ref="E10:E11" si="1">D10/1505</f>
+        <f t="shared" ref="E10:E11" si="5">D10/1505</f>
         <v>47.270544850498339</v>
       </c>
       <c r="F10" s="17">
@@ -1965,7 +2471,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="18">
-        <f>B10+C10+E10-F10-G10</f>
+        <f t="shared" ref="H10:H12" si="6">B10+C10+E10-F10-G10</f>
         <v>271.42054485049835</v>
       </c>
       <c r="I10" s="19">
@@ -1979,11 +2485,11 @@
         <v>53.899999999999999</v>
       </c>
       <c r="L10" s="22">
-        <f>K10-J10</f>
+        <f t="shared" ref="L10:L12" si="7">K10-J10</f>
         <v>-36.573514950166121</v>
       </c>
       <c r="M10" s="23">
-        <f>J10*100/K10</f>
+        <f t="shared" ref="M10:M12" si="8">J10*100/K10</f>
         <v>167.85438766264588</v>
       </c>
     </row>
@@ -1997,13 +2503,13 @@
       <c r="C11" s="26"/>
       <c r="D11" s="27"/>
       <c r="E11" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
       <c r="H11" s="18">
-        <f>B11+C11+E11-F11-G11</f>
+        <f t="shared" si="6"/>
         <v>159.80000000000001</v>
       </c>
       <c r="I11" s="19">
@@ -2014,11 +2520,11 @@
         <v>73.900000000000006</v>
       </c>
       <c r="L11" s="22">
-        <f>K11-J11</f>
+        <f t="shared" si="7"/>
         <v>73.900000000000006</v>
       </c>
       <c r="M11" s="23">
-        <f>J11*100/K11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -2041,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="18">
-        <f>B12+C12+E12-F12-G12</f>
+        <f t="shared" si="6"/>
         <v>307.97000000000003</v>
       </c>
       <c r="I12" s="19">
@@ -2055,11 +2561,11 @@
         <v>77.159999999999997</v>
       </c>
       <c r="L12" s="22">
-        <f>K12-J12</f>
+        <f t="shared" si="7"/>
         <v>-25.496666666666684</v>
       </c>
       <c r="M12" s="23">
-        <f>J12*100/K12</f>
+        <f t="shared" si="8"/>
         <v>133.0438914809055</v>
       </c>
     </row>
@@ -2097,4 +2603,641 @@
   <headerFooter/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView topLeftCell="A6" zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" style="29" width="11.2421875"/>
+    <col bestFit="1" min="2" max="2" style="29" width="12.47265625"/>
+    <col bestFit="1" min="3" max="3" style="29" width="10.83203125"/>
+    <col bestFit="1" min="4" max="4" style="30" width="95.8125"/>
+    <col min="5" max="16384" style="29" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="34">
+        <v>1</v>
+      </c>
+      <c r="C2" s="35">
+        <v>45995</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="37"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="38">
+        <v>46002</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="37"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="38">
+        <v>46024</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="38">
+        <v>46028</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="37"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="40">
+        <v>46030</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="34">
+        <v>2</v>
+      </c>
+      <c r="C7" s="35">
+        <v>45999</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="37"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="38">
+        <v>46002</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="37"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="38">
+        <v>46007</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="37"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="38">
+        <v>46013</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="37"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="38">
+        <v>46020</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="43">
+        <v>3</v>
+      </c>
+      <c r="C12" s="35">
+        <v>46031</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="38">
+        <v>46035</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="38">
+        <v>46038</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="45"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="40">
+        <v>46043</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" ht="28.5">
+      <c r="A16" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="34">
+        <v>1</v>
+      </c>
+      <c r="C16" s="38">
+        <v>45995</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="49"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="38">
+        <v>46020</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="49"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" ht="28.5">
+      <c r="A19" s="49"/>
+      <c r="B19" s="34">
+        <v>2</v>
+      </c>
+      <c r="C19" s="35">
+        <v>46021</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="49"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="38">
+        <v>46031</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="49"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="38">
+        <v>46042</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="43">
+        <v>1</v>
+      </c>
+      <c r="C22" s="35">
+        <v>46031</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="45"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="53"/>
+    </row>
+    <row r="24" ht="28.5">
+      <c r="A24" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="34">
+        <v>1</v>
+      </c>
+      <c r="C24" s="38">
+        <v>45995</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" ht="28.5">
+      <c r="A25" s="48"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="40">
+        <v>46017</v>
+      </c>
+      <c r="D25" s="47" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" ht="28.5">
+      <c r="A26" s="48"/>
+      <c r="B26" s="34">
+        <v>2</v>
+      </c>
+      <c r="C26" s="35">
+        <v>45995</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" ht="28.5">
+      <c r="A27" s="48"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="40">
+        <v>46020</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="48"/>
+      <c r="B28" s="34">
+        <v>3</v>
+      </c>
+      <c r="C28" s="35">
+        <v>46021</v>
+      </c>
+      <c r="D28" s="51" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" ht="28.5">
+      <c r="A29" s="48"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="38">
+        <v>46029</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="34">
+        <v>1</v>
+      </c>
+      <c r="C30" s="35">
+        <v>45995</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" s="49"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="38">
+        <v>46002</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" s="49"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="38">
+        <v>46006</v>
+      </c>
+      <c r="D32" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" s="49"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="38">
+        <v>46013</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="A34" s="55"/>
+      <c r="B34" s="56">
+        <v>2</v>
+      </c>
+      <c r="C34" s="57">
+        <v>45999</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35" s="55"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="59">
+        <v>46004</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" s="55"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="59">
+        <v>46009</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" s="55"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="59">
+        <v>46013</v>
+      </c>
+      <c r="D37" s="39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" s="55"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="59">
+        <v>46020</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" s="55"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="59">
+        <v>46038</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40" s="55"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="A41" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="56">
+        <v>1</v>
+      </c>
+      <c r="C41" s="35">
+        <v>46001</v>
+      </c>
+      <c r="D41" s="51" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" ht="14.25">
+      <c r="A42" s="63"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="38">
+        <v>46002</v>
+      </c>
+      <c r="D42" s="39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" ht="14.25">
+      <c r="A43" s="63"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="40">
+        <v>46017</v>
+      </c>
+      <c r="D43" s="41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" ht="14.25">
+      <c r="A44" s="63"/>
+      <c r="B44" s="64">
+        <v>2</v>
+      </c>
+      <c r="C44" s="35">
+        <v>46029</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" ht="14.25">
+      <c r="A45" s="63"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="38">
+        <v>46030</v>
+      </c>
+      <c r="D45" s="39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25">
+      <c r="A46" s="63"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="38">
+        <v>46034</v>
+      </c>
+      <c r="D46" s="39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25">
+      <c r="A47" s="65"/>
+      <c r="B47" s="66"/>
+      <c r="C47" s="40">
+        <v>46372</v>
+      </c>
+      <c r="D47" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" ht="14.25">
+      <c r="A48" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" s="56">
+        <v>1</v>
+      </c>
+      <c r="C48" s="35">
+        <v>46001</v>
+      </c>
+      <c r="D48" s="36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" ht="14.25">
+      <c r="A49" s="63"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="38">
+        <v>46009</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" ht="14.25">
+      <c r="A50" s="63"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="38">
+        <v>46013</v>
+      </c>
+      <c r="D50" s="39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" ht="14.25">
+      <c r="A51" s="63"/>
+      <c r="B51" s="58"/>
+      <c r="C51" s="38">
+        <v>46015</v>
+      </c>
+      <c r="D51" s="42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" ht="14.25">
+      <c r="A52" s="63"/>
+      <c r="B52" s="58"/>
+      <c r="C52" s="38">
+        <v>46017</v>
+      </c>
+      <c r="D52" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" ht="14.25">
+      <c r="A53" s="63"/>
+      <c r="B53" s="58"/>
+      <c r="C53" s="38">
+        <v>46022</v>
+      </c>
+      <c r="D53" s="39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" ht="14.25">
+      <c r="A54" s="63"/>
+      <c r="B54" s="58"/>
+      <c r="C54" s="38">
+        <v>46027</v>
+      </c>
+      <c r="D54" s="39" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" ht="14.25">
+      <c r="A55" s="65"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="40">
+        <v>46034</v>
+      </c>
+      <c r="D55" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A40"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A48:A55"/>
+    <mergeCell ref="B48:B55"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>